<commit_message>
Fix config for sender name
</commit_message>
<xml_diff>
--- a/Data/Config dev.xlsx
+++ b/Data/Config dev.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\Kalyana\Traveloka_DataAutomation_UploadBucket\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tvlk\upload bucket local repo\add-new-queue-item repo\Upload_Bucket\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF23F71-1263-4398-ACFC-A041D27D85D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F638260-8FA3-4680-8603-606A8049C5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
-    <t>Email_SenderName</t>
+    <t>EmailSenderName</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update mark log tested
</commit_message>
<xml_diff>
--- a/Data/Config dev.xlsx
+++ b/Data/Config dev.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tvlk\upload bucket local repo\add-new-queue-item repo\Upload_Bucket\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Upload_Bucket\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F638260-8FA3-4680-8603-606A8049C5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FDD9DA-98D5-4101-9E58-0FD242B0DD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="14520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>RPA_Moon_AWS_Region</t>
   </si>
   <si>
-    <t>RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
     <t>AWS_SQS_QueueName</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>EmailSenderName</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathMailTemplate</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -2834,7 +2834,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2886,7 +2886,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2894,7 +2894,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2910,23 +2910,23 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>